<commit_message>
added new parts and reorg
</commit_message>
<xml_diff>
--- a/3D Prints/Print Tracking.xlsx
+++ b/3D Prints/Print Tracking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esher\Desktop\Desktop\robotic-arm\3D Prints\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE847B54-B90F-4910-8BAF-5CC5A4AD7E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD1C860-905A-41C7-AE3A-EB8FA0509365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
   <si>
     <t>Printed By</t>
   </si>
@@ -69,7 +69,19 @@
     <t>Print File Name in Folder</t>
   </si>
   <si>
-    <t>Slicer Used</t>
+    <t>Nathan</t>
+  </si>
+  <si>
+    <t>sort of</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>main wrist new</t>
+  </si>
+  <si>
+    <t>tricep</t>
   </si>
 </sst>
 </file>
@@ -401,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,12 +424,12 @@
     <col min="1" max="1" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5703125" customWidth="1"/>
-    <col min="4" max="5" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -431,77 +443,138 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>3</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>2</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>5</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>